<commit_message>
Updated v3.5.1 Medication and Procedure Defined Lists for blood product administration.
</commit_message>
<xml_diff>
--- a/DefinedLists/Medication/Medication.xlsx
+++ b/DefinedLists/Medication/Medication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\NEMSIS\NEMSIS V3\Defined and Suggested Lists for v3.5.0\Defined and Suggested Lists Most Current\Defined\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\NEMSIS TAC\Repository\nemsis_public\DefinedLists\Medication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BBFD9C-52B4-4FF9-8E1C-6D65A7CE011C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9964563D-C0E7-4A23-9EEC-7F981E58DC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recommendation" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
   <si>
     <t>NOTES</t>
   </si>
@@ -422,9 +422,6 @@
   </si>
   <si>
     <t>Transfusion of fresh frozen plasma </t>
-  </si>
-  <si>
-    <t>Fresh frozen plasma (FFP)</t>
   </si>
   <si>
     <t>EMS DESCRIPTION (Acronym)</t>
@@ -475,11 +472,23 @@
     <t>Added 07/08/2024</t>
   </si>
   <si>
-    <t>Most Recent Update: 07/08/2024
+    <t>Added</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Plasma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 See Change Log tab for details</t>
   </si>
   <si>
-    <t>Added</t>
+    <t>"fresh frozen" removed from EMS Description 01/15/2025</t>
+  </si>
+  <si>
+    <t>SNOMED CT code 116861002 - removed fresh frozen from EMS Description 01/15/2025</t>
   </si>
 </sst>
 </file>
@@ -1055,43 +1064,39 @@
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1109,11 +1114,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1132,16 +1133,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1150,39 +1148,39 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1553,853 +1551,790 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="63.140625" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="1" max="1" width="40.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="63.109375" customWidth="1"/>
+    <col min="4" max="4" width="82.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="37"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="36" t="s">
-        <v>145</v>
+    <row r="1" spans="1:7" s="19" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="32"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="31" t="s">
+        <v>147</v>
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
       <c r="C3" s="2"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>161</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="23"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>296</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="23"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>435</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="23"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>214199</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="23"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>703</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="23"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>1191</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="23"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>1223</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="23"/>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1819</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="7">
-        <v>1819</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>1901</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="23"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>1908</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="23"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="4">
         <v>2193</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="23"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>3264</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>1795477</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="23"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>260258</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="23"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>237653</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="23"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>3322</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="23"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>3443</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="23"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>3498</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="23"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>3628</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="23"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>328316</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="23"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>317361</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="23"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>4177</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="23"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>4337</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="23"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>4603</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="23"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>4832</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="23"/>
-    </row>
-    <row r="32" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <v>4850</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="19"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="D32" s="17"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>5093</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="23"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <v>5224</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="23"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>3423</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="23"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>1605101</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="23"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <v>7213</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="23"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <v>6130</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="23"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="6">
         <v>35827</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="23"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="6">
         <v>6185</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="23"/>
-    </row>
-    <row r="41" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+    </row>
+    <row r="41" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="13">
         <v>1008377</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="6">
         <v>237159</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="23"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="6">
         <v>6387</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="23"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <v>6470</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="23"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="6">
         <v>6585</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="23"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="6">
         <v>6902</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="23"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="6">
         <v>6918</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="23"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <v>6960</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="23"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="6">
         <v>7052</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="23"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="6">
         <v>7242</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="23"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="6">
         <v>7396</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="23"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="6">
         <v>4917</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="D52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="6">
         <v>7512</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D53" s="23"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="6">
         <v>26225</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="23"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="6">
         <v>7806</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D55" s="23"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="6">
         <v>8163</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="23"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="6">
         <v>8591</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D57" s="23"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="6">
         <v>8745</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D58" s="23"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="6">
         <v>8782</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D59" s="23"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="6">
         <v>68139</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="23"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="6">
         <v>36676</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D61" s="23"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="38">
+      <c r="B62" s="33">
         <v>313002</v>
       </c>
-      <c r="C62" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D62" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="E62" s="14"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="13"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="C62" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" t="s">
+        <v>140</v>
+      </c>
+      <c r="E62" s="12"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="6">
         <v>10154</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D63" s="23"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="6">
         <v>10368</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D64" s="23"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="6">
         <v>10454</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D65" s="23"/>
-    </row>
-    <row r="66" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="32" t="s">
+    </row>
+    <row r="66" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="33">
+      <c r="B66" s="28">
         <v>10691</v>
       </c>
-      <c r="C66" s="34" t="s">
+      <c r="C66" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="4">
         <v>11124</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D67" s="23"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="6">
         <v>11149</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D68" s="23"/>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
+    </row>
+    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="6">
         <v>71535</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D69" s="23"/>
-    </row>
-    <row r="70" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B70" s="28" t="s">
+    </row>
+    <row r="70" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B70" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="C70" s="29" t="s">
+      <c r="C70" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D70" s="30" t="s">
+      <c r="D70" s="26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>125</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B71" s="4">
         <v>116762002</v>
       </c>
       <c r="C71" t="s">
@@ -2409,80 +2344,77 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B72" s="4">
         <v>116795008</v>
       </c>
       <c r="C72" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B73" s="31">
+    <row r="73" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" s="28">
         <v>116861002</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="C73" s="14" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="D73" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>128</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="4">
         <v>116865006</v>
       </c>
       <c r="C74" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>129</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="4">
         <v>180208003</v>
       </c>
       <c r="C75" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>126</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="4">
         <v>33389009</v>
       </c>
       <c r="C76" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>130</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="4">
         <v>71493000</v>
       </c>
       <c r="C77" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
-    </row>
   </sheetData>
-  <sortState ref="G1:G4">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G4">
     <sortCondition ref="G1"/>
   </sortState>
   <mergeCells count="1">
@@ -2498,80 +2430,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="5" width="112.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="112.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="37" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="36">
+        <v>44155</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="35">
+        <v>313002</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="41">
-        <v>44155</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="40">
-        <v>313002</v>
-      </c>
-      <c r="D2" s="44" t="s">
+      <c r="E2" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="43" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="47">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="40">
         <v>45481</v>
       </c>
-      <c r="B3" s="48" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="49">
+      <c r="B3" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="42">
         <v>1819</v>
       </c>
-      <c r="D3" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="35" t="s">
+      <c r="D3" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="43">
+        <v>45672</v>
+      </c>
+      <c r="B4" t="s">
         <v>146</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1">
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>